<commit_message>
refactoring factory method pattern
</commit_message>
<xml_diff>
--- a/data/news_category.xlsx
+++ b/data/news_category.xlsx
@@ -4,23 +4,24 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="politics"/>
-    <sheet r:id="rId2" sheetId="2" name="economy"/>
-    <sheet r:id="rId3" sheetId="3" name="international"/>
-    <sheet r:id="rId4" sheetId="4" name="society"/>
-    <sheet r:id="rId5" sheetId="5" name="culture"/>
-    <sheet r:id="rId6" sheetId="6" name="entertainment"/>
-    <sheet r:id="rId7" sheetId="7" name="sports"/>
+    <sheet r:id="rId1" sheetId="1" name="hankook"/>
+    <sheet r:id="rId2" sheetId="2" name="politics"/>
+    <sheet r:id="rId3" sheetId="3" name="economy"/>
+    <sheet r:id="rId4" sheetId="4" name="international"/>
+    <sheet r:id="rId5" sheetId="5" name="society"/>
+    <sheet r:id="rId6" sheetId="6" name="culture"/>
+    <sheet r:id="rId7" sheetId="7" name="entertainment"/>
+    <sheet r:id="rId8" sheetId="8" name="sports"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="337">
   <si>
     <t>chosun</t>
   </si>
@@ -454,6 +455,9 @@
     <t>law</t>
   </si>
   <si>
+    <t>Series/70030000000923</t>
+  </si>
+  <si>
     <t>education</t>
   </si>
   <si>
@@ -583,6 +587,12 @@
     <t>reigonal</t>
   </si>
   <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
     <t>international</t>
   </si>
   <si>
@@ -598,6 +608,9 @@
     <t>World</t>
   </si>
   <si>
+    <t>sub1</t>
+  </si>
+  <si>
     <t>international_general</t>
   </si>
   <si>
@@ -613,6 +626,9 @@
     <t>HD01</t>
   </si>
   <si>
+    <t>sub2</t>
+  </si>
+  <si>
     <t>us</t>
   </si>
   <si>
@@ -634,6 +650,9 @@
     <t>HD02</t>
   </si>
   <si>
+    <t>sub3</t>
+  </si>
+  <si>
     <t>china</t>
   </si>
   <si>
@@ -649,6 +668,9 @@
     <t>HD03</t>
   </si>
   <si>
+    <t>sub4</t>
+  </si>
+  <si>
     <t>EU</t>
   </si>
   <si>
@@ -658,6 +680,9 @@
     <t>HD04</t>
   </si>
   <si>
+    <t>sub5</t>
+  </si>
+  <si>
     <t>asia</t>
   </si>
   <si>
@@ -679,6 +704,9 @@
     <t>HD05</t>
   </si>
   <si>
+    <t>sub</t>
+  </si>
+  <si>
     <t>euorpe</t>
   </si>
   <si>
@@ -715,12 +743,12 @@
     <t>globaleconomy</t>
   </si>
   <si>
+    <t>money</t>
+  </si>
+  <si>
     <t>economy</t>
   </si>
   <si>
-    <t>money</t>
-  </si>
-  <si>
     <t>Economy</t>
   </si>
   <si>
@@ -799,6 +827,9 @@
     <t>HB05</t>
   </si>
   <si>
+    <t>sub6</t>
+  </si>
+  <si>
     <t>industry-company</t>
   </si>
   <si>
@@ -820,6 +851,9 @@
     <t>HB99</t>
   </si>
   <si>
+    <t>sub7</t>
+  </si>
+  <si>
     <t>market_trend</t>
   </si>
   <si>
@@ -832,6 +866,9 @@
     <t>it</t>
   </si>
   <si>
+    <t>sub8</t>
+  </si>
+  <si>
     <t>startup_story</t>
   </si>
   <si>
@@ -841,12 +878,18 @@
     <t>working</t>
   </si>
   <si>
+    <t>sub9</t>
+  </si>
+  <si>
     <t>policy</t>
   </si>
   <si>
     <t>startup</t>
   </si>
   <si>
+    <t>sub10</t>
+  </si>
+  <si>
     <t>smb-venture</t>
   </si>
   <si>
@@ -856,13 +899,22 @@
     <t>biznews</t>
   </si>
   <si>
+    <t>sub11</t>
+  </si>
+  <si>
     <t>stock-finance</t>
   </si>
   <si>
     <t>global</t>
   </si>
   <si>
+    <t>sub12</t>
+  </si>
+  <si>
     <t>tech_it</t>
+  </si>
+  <si>
+    <t>sub13</t>
   </si>
   <si>
     <t>weeklybiz</t>
@@ -987,7 +1039,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1011,6 +1063,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1041,13 +1099,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1061,7 +1116,25 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1366,24 +1439,164 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1410,208 +1623,208 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>189</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C3" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>284</v>
+      <c r="E3" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>301</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+        <v>201</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+        <v>209</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+        <v>215</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+        <v>219</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>317</v>
+        <v>268</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>310</v>
+      <c r="F8" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>327</v>
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>276</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1619,8 +1832,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="4" t="s">
-        <v>319</v>
+      <c r="H9" s="3" t="s">
+        <v>336</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -1629,7 +1842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1641,18 +1854,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="36.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
-      <c r="A1" s="1"/>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="6" t="s">
+        <v>240</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1678,316 +1893,316 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="12" t="s">
+        <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C3" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="E3" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D4" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
-      <c r="A6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
-      <c r="A7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
-      <c r="A8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
-      <c r="A9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
-      <c r="A10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
-      <c r="A11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="4" t="s">
-        <v>273</v>
+      <c r="E11" s="3" t="s">
+        <v>286</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="4" t="s">
-        <v>274</v>
+      <c r="H11" s="3" t="s">
+        <v>287</v>
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
-      <c r="A12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>275</v>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>289</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="4" t="s">
-        <v>276</v>
+      <c r="E12" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="4" t="s">
-        <v>277</v>
+      <c r="H12" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>278</v>
+        <v>292</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="4" t="s">
-        <v>279</v>
+      <c r="H13" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
-      <c r="A14" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>280</v>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>296</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1997,12 +2212,12 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>281</v>
+        <v>297</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2017,7 +2232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -2028,19 +2243,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
-      <c r="A1" s="1"/>
+      <c r="A1" s="8" t="s">
+        <v>188</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2067,273 +2284,273 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="9" t="s">
+        <v>189</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>187</v>
-      </c>
       <c r="I2" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="E3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>196</v>
       </c>
+      <c r="I3" s="3" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>203</v>
+      <c r="H4" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="A5" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+      <c r="A6" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
-      <c r="A6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="C6" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+      <c r="A7" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+      <c r="A8" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
-      <c r="A7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
-      <c r="A8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>223</v>
+      <c r="I8" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
-      <c r="A9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>224</v>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>226</v>
+      <c r="E9" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="4" t="s">
-        <v>201</v>
+      <c r="H9" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>206</v>
+      <c r="B10" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="4" t="s">
-        <v>217</v>
+      <c r="E10" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="4" t="s">
-        <v>227</v>
+      <c r="H10" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="4" t="s">
-        <v>193</v>
+      <c r="E11" s="3" t="s">
+        <v>197</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="4" t="s">
-        <v>228</v>
+      <c r="H11" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="10" t="s">
         <v>118</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="3" t="s">
-        <v>229</v>
+      <c r="E12" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="4" t="s">
-        <v>230</v>
+      <c r="H12" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -2342,30 +2559,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="42.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
-      <c r="A1" s="1"/>
+      <c r="A1" s="6"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2424,28 +2641,28 @@
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2453,28 +2670,28 @@
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2482,165 +2699,165 @@
       <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>147</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
       <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>150</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
       <c r="A7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="E7" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>156</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
       <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>164</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
       <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>149</v>
+      <c r="B9" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="G9" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>169</v>
+      <c r="I9" s="3" t="s">
+        <v>170</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
       <c r="A10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>171</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>172</v>
+      <c r="E10" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="4" t="s">
-        <v>161</v>
+      <c r="H10" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="I10" s="1"/>
     </row>
@@ -2648,18 +2865,18 @@
       <c r="A11" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>130</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="4" t="s">
-        <v>174</v>
+      <c r="H11" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -2667,16 +2884,16 @@
       <c r="A12" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>175</v>
+      <c r="B12" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="4" t="s">
-        <v>176</v>
+      <c r="H12" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -2684,16 +2901,16 @@
       <c r="A13" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>177</v>
+      <c r="B13" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="4" t="s">
-        <v>178</v>
+      <c r="H13" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="I13" s="1"/>
     </row>
@@ -2701,16 +2918,16 @@
       <c r="A14" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>179</v>
+      <c r="B14" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="4" t="s">
-        <v>180</v>
+      <c r="H14" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -2718,16 +2935,16 @@
       <c r="A15" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>181</v>
+      <c r="B15" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="4" t="s">
-        <v>182</v>
+      <c r="H15" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -2735,25 +2952,25 @@
       <c r="A16" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>183</v>
+      <c r="B16" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="4" t="s">
-        <v>184</v>
+      <c r="H16" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="I16" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
       <c r="A17" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="B17" s="4" t="s">
         <v>186</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2768,7 +2985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -2780,18 +2997,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
-      <c r="A1" s="1"/>
+      <c r="A1" s="6"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2850,28 +3067,28 @@
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2879,28 +3096,28 @@
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2908,28 +3125,28 @@
       <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2937,25 +3154,25 @@
       <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>101</v>
       </c>
       <c r="I6" s="1"/>
@@ -2964,25 +3181,25 @@
       <c r="A7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>75</v>
       </c>
       <c r="I7" s="1"/>
@@ -2991,23 +3208,23 @@
       <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>109</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>99</v>
       </c>
       <c r="I8" s="1"/>
@@ -3016,21 +3233,21 @@
       <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>65</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>85</v>
       </c>
       <c r="I9" s="1"/>
@@ -3039,34 +3256,34 @@
       <c r="A10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>114</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="3"/>
       <c r="I10" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
       <c r="A11" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>115</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>117</v>
       </c>
       <c r="G11" s="1"/>
@@ -3077,12 +3294,12 @@
       <c r="A12" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>119</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>120</v>
       </c>
       <c r="F12" s="1"/>
@@ -3094,12 +3311,12 @@
       <c r="A13" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>122</v>
       </c>
       <c r="F13" s="1"/>
@@ -3111,12 +3328,12 @@
       <c r="A14" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>125</v>
       </c>
       <c r="F14" s="1"/>
@@ -3128,12 +3345,12 @@
       <c r="A15" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>88</v>
       </c>
       <c r="F15" s="1"/>
@@ -3145,7 +3362,7 @@
       <c r="A16" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C16" s="1"/>
@@ -3155,211 +3372,6 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.005" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
-      <c r="A2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
-      <c r="A3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
-      <c r="A5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
-      <c r="A6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
-      <c r="A7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
-      <c r="A8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
-        <v>80</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3371,21 +3383,226 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.005" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+      <c r="A1" s="6"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+      <c r="A5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+      <c r="A6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+      <c r="A7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+      <c r="A8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
@@ -3448,28 +3665,28 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3477,28 +3694,28 @@
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3506,28 +3723,28 @@
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3535,28 +3752,28 @@
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3564,28 +3781,28 @@
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3593,24 +3810,24 @@
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3618,20 +3835,20 @@
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3639,7 +3856,7 @@
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="1"/>
@@ -3647,7 +3864,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>52</v>
       </c>
       <c r="I10" s="1"/>
@@ -3656,7 +3873,7 @@
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="1"/>

</xml_diff>